<commit_message>
Flujos de refinanciacion Especial y registro de informe vista verificacion
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoEmpresarialRefinanciacionEspecial.xlsx
+++ b/target/DatosExcel/DatosCreditoEmpresarialRefinanciacionEspecial.xlsx
@@ -86,9 +86,6 @@
     <t>SubTipo Propuesta</t>
   </si>
   <si>
-    <t>1332236</t>
-  </si>
-  <si>
     <t>REFINANCIACION ESPECIAL</t>
   </si>
   <si>
@@ -123,6 +120,9 @@
   </si>
   <si>
     <t>EFECTIVO</t>
+  </si>
+  <si>
+    <t>3534375</t>
   </si>
 </sst>
 </file>
@@ -459,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -500,13 +500,13 @@
         <v>12</v>
       </c>
       <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
       <c r="I1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J1" t="s">
         <v>2</v>
@@ -515,13 +515,13 @@
         <v>3</v>
       </c>
       <c r="L1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M1" t="s">
         <v>14</v>
       </c>
       <c r="N1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O1" t="s">
         <v>4</v>
@@ -538,7 +538,7 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
@@ -547,7 +547,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
@@ -556,34 +556,34 @@
         <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="N2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Avance del registro Informe de Visita Verificacion jefe credito
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoEmpresarialRefinanciacionEspecial.xlsx
+++ b/target/DatosExcel/DatosCreditoEmpresarialRefinanciacionEspecial.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>Cliente</t>
   </si>
@@ -122,14 +122,26 @@
     <t>EFECTIVO</t>
   </si>
   <si>
+    <t>NroPropuesta</t>
+  </si>
+  <si>
     <t>3534375</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>19499545</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +155,14 @@
       <color rgb="FF297BDE"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -171,12 +191,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -478,9 +499,10 @@
     <col min="16" max="16" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="30" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="30" customWidth="1"/>
+    <col min="19" max="19" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -535,10 +557,13 @@
       <c r="R1" t="s">
         <v>16</v>
       </c>
+      <c r="S1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:19">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
@@ -591,6 +616,65 @@
       <c r="R2" s="2" t="s">
         <v>8</v>
       </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="N9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Avance de escritura excel
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoEmpresarialRefinanciacionEspecial.xlsx
+++ b/target/DatosExcel/DatosCreditoEmpresarialRefinanciacionEspecial.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>Cliente</t>
   </si>
@@ -122,19 +122,25 @@
     <t>EFECTIVO</t>
   </si>
   <si>
-    <t>NroPropuesta</t>
-  </si>
-  <si>
     <t>3534375</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>19499545</t>
-  </si>
-  <si>
-    <t>6</t>
+    <t>prueba</t>
+  </si>
+  <si>
+    <t>Numero Propuesta</t>
+  </si>
+  <si>
+    <t>Observacion</t>
+  </si>
+  <si>
+    <t>contrasena</t>
+  </si>
+  <si>
+    <t>Aprobado</t>
+  </si>
+  <si>
+    <t>gggg</t>
   </si>
 </sst>
 </file>
@@ -478,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7:T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -499,10 +505,10 @@
     <col min="16" max="16" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="30" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="30" customWidth="1"/>
-    <col min="19" max="19" width="13.28515625" customWidth="1"/>
+    <col min="21" max="21" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -558,12 +564,18 @@
         <v>16</v>
       </c>
       <c r="S1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" s="2" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
@@ -616,65 +628,18 @@
       <c r="R2" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="S2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="3" spans="1:19">
-      <c r="A3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19">
-      <c r="N9" s="3"/>
+    <row r="8" spans="1:21">
+      <c r="N8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Version corregida de la integracion refinanciacion y reprogramacion
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoEmpresarialRefinanciacionEspecial.xlsx
+++ b/target/DatosExcel/DatosCreditoEmpresarialRefinanciacionEspecial.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CajaPiuraCMAC2021\target\DatosExcel\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
   <si>
     <t>Cliente</t>
   </si>
@@ -122,9 +122,6 @@
     <t>EFECTIVO</t>
   </si>
   <si>
-    <t>3534375</t>
-  </si>
-  <si>
     <t>prueba</t>
   </si>
   <si>
@@ -140,13 +137,26 @@
     <t>Aprobado</t>
   </si>
   <si>
-    <t>gggg</t>
+    <t>5802202</t>
+  </si>
+  <si>
+    <t>19499545</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>4873648</t>
+  </si>
+  <si>
+    <t>4873649</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -487,25 +497,25 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7:T7"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" customWidth="1"/>
-    <col min="11" max="14" width="19.42578125" customWidth="1"/>
-    <col min="15" max="15" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="30" customWidth="1"/>
-    <col min="21" max="21" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="13.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -564,18 +574,18 @@
         <v>16</v>
       </c>
       <c r="S1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T1" t="s">
         <v>35</v>
       </c>
-      <c r="T1" t="s">
-        <v>36</v>
-      </c>
       <c r="U1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:21">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
@@ -629,13 +639,78 @@
         <v>8</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="U2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" s="2" t="s">
         <v>38</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:21">

</xml_diff>

<commit_message>
Guardar el resultado de emision de la propuesta
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoEmpresarialRefinanciacionEspecial.xlsx
+++ b/target/DatosExcel/DatosCreditoEmpresarialRefinanciacionEspecial.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CajaPiuraCMAC2021\target\DatosExcel\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>Cliente</t>
   </si>
@@ -137,26 +137,22 @@
     <t>Aprobado</t>
   </si>
   <si>
-    <t>5802202</t>
-  </si>
-  <si>
     <t>19499545</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>4873648</t>
-  </si>
-  <si>
-    <t>4873649</t>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>4873658</t>
+  </si>
+  <si>
+    <t>Se han encontrado errores en la Validacion de la Propuesta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -207,13 +203,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,31 +491,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="11" max="14" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="14" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="30" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="61.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -582,8 +580,11 @@
       <c r="U1" t="s">
         <v>33</v>
       </c>
+      <c r="V1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:22">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -644,77 +645,15 @@
       <c r="T2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
-      <c r="A3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21">
-      <c r="N8" s="3"/>
+    <row r="7" spans="1:22">
+      <c r="N7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cambios en la integracion de reprogramacion
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoEmpresarialRefinanciacionEspecial.xlsx
+++ b/target/DatosExcel/DatosCreditoEmpresarialRefinanciacionEspecial.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>Cliente</t>
   </si>
@@ -116,9 +116,6 @@
     <t>Cuotas</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>EFECTIVO</t>
   </si>
   <si>
@@ -143,25 +140,13 @@
     <t>Resultado</t>
   </si>
   <si>
-    <t>40289</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>6</t>
   </si>
   <si>
-    <t>4873665</t>
-  </si>
-  <si>
-    <t>4873666</t>
+    <t>4873680</t>
   </si>
   <si>
     <t>El Documento ha sido derivado satisfactoriamente</t>
-  </si>
-  <si>
-    <t>Se han encontrado errores en la Validacion de la Propuesta</t>
   </si>
 </sst>
 </file>
@@ -509,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -588,21 +573,21 @@
         <v>16</v>
       </c>
       <c r="S1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T1" t="s">
         <v>34</v>
       </c>
-      <c r="T1" t="s">
-        <v>35</v>
-      </c>
       <c r="U1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
@@ -641,13 +626,13 @@
         <v>28</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>8</v>
@@ -656,84 +641,16 @@
         <v>8</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U2" t="s">
-        <v>42</v>
+        <v>31</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="V2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22">
-      <c r="A3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U3" t="s">
-        <v>43</v>
-      </c>
-      <c r="V3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:22">

</xml_diff>

<commit_message>
Version modificada para el informe tecnico
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoEmpresarialRefinanciacionEspecial.xlsx
+++ b/target/DatosExcel/DatosCreditoEmpresarialRefinanciacionEspecial.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CajaPiuraCMAC2021\target\DatosExcel\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>Cliente</t>
   </si>
@@ -134,16 +134,28 @@
     <t>Aprobado</t>
   </si>
   <si>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>3534375</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
     <t>19499545</t>
   </si>
   <si>
-    <t>Resultado</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>4873680</t>
+    <t>4873741</t>
+  </si>
+  <si>
+    <t>4873742</t>
   </si>
   <si>
     <t>El Documento ha sido derivado satisfactoriamente</t>
@@ -153,7 +165,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -178,7 +189,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,6 +199,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -204,14 +221,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,167 +514,237 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="11" max="14" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="61.7109375" collapsed="true"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="12" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="30" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="33.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
-      <c r="A1" t="s">
+    <row r="1" spans="1:22" s="4" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" s="4" customFormat="1">
+      <c r="A2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>37</v>
       </c>
+      <c r="O2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:22">
-      <c r="A2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="1:22" s="4" customFormat="1">
+      <c r="A3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="H3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="O2" s="2" t="s">
+      <c r="N3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="T3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="U2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="V2" t="s">
-        <v>40</v>
+      <c r="U3" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:22">
-      <c r="N7" s="3"/>
+      <c r="N7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>